<commit_message>
Enhanced charts for the streamlit app.
</commit_message>
<xml_diff>
--- a/Mash3_BGS_Talk_v01.xlsx
+++ b/Mash3_BGS_Talk_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\Matias\Proyectos personales\Mash3_simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA3282B-37DA-4561-8647-B616340B7E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A865274F-F438-4AA2-9D5D-1EE8D674FA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2115" yWindow="2115" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1678,10 +1678,10 @@
   <dimension ref="A1:AG45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -2435,7 +2435,7 @@
         <v>467.1875</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" ref="E16:P16" si="2">(F26*F33)+(F43*F37)</f>
+        <f t="shared" ref="G16:P16" si="2">(F26*F33)+(F43*F37)</f>
         <v>513.41796875</v>
       </c>
       <c r="H16" s="9">
@@ -3731,7 +3731,7 @@
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
       <c r="D29" s="36">
-        <f t="shared" ref="D29:P29" si="24">D26</f>
+        <f t="shared" ref="D29" si="24">D26</f>
         <v>1500</v>
       </c>
       <c r="E29" s="36">

</xml_diff>